<commit_message>
Added workflow to get Current IST
</commit_message>
<xml_diff>
--- a/SearchKeywords.xlsx
+++ b/SearchKeywords.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\RPA_UIPATH\UIPath-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27B3D2B3-6E05-48EC-BA86-D3790D0FEEBD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00B55EBD-BB01-46D1-8A28-75E5B4F5E870}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{1248EEDB-3F50-4913-B01C-A4A23D5E2DC7}"/>
   </bookViews>
@@ -20,26 +20,29 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Search Terms</t>
   </si>
   <si>
+    <t>Search Result</t>
+  </si>
+  <si>
     <t>Selenium</t>
   </si>
   <si>
+    <t>www.selenium.dev</t>
+  </si>
+  <si>
     <t>RPA-UI Path</t>
+  </si>
+  <si>
+    <t>www.uipath.com</t>
   </si>
 </sst>
 </file>
@@ -75,8 +78,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -391,30 +395,40 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DA5586B-81F5-43A1-9130-F6AF939199A0}">
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.21875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>1</v>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>2</v>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>